<commit_message>
Submitted info on backlog
</commit_message>
<xml_diff>
--- a/agile/sprint2.xlsx
+++ b/agile/sprint2.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Google Drive\Git\fanorona12\agile\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="sprint2_backlog" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>id</t>
   </si>
@@ -99,7 +94,7 @@
     <t>projection</t>
   </si>
   <si>
-    <t>M</t>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -637,9 +632,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -751,11 +743,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1433156528"/>
-        <c:axId val="-1433160880"/>
+        <c:axId val="95866816"/>
+        <c:axId val="95867392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1433156528"/>
+        <c:axId val="95866816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -784,12 +776,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1433160880"/>
+        <c:crossAx val="95867392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1433160880"/>
+        <c:axId val="95867392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -824,7 +816,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1433156528"/>
+        <c:crossAx val="95866816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -924,7 +916,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -959,7 +951,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1171,7 +1163,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,12 +1214,6 @@
       <c r="C2">
         <v>120</v>
       </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2">
-        <v>120</v>
-      </c>
       <c r="I2">
         <v>0</v>
       </c>
@@ -1261,12 +1247,6 @@
       <c r="C3">
         <v>30</v>
       </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3">
-        <v>20</v>
-      </c>
       <c r="J3">
         <v>0</v>
       </c>
@@ -1361,6 +1341,15 @@
       <c r="C7">
         <v>60</v>
       </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7">
+        <v>180</v>
+      </c>
       <c r="J7">
         <v>0</v>
       </c>
@@ -1416,12 +1405,6 @@
       <c r="C10">
         <v>20</v>
       </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10">
-        <v>20</v>
-      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1433,12 +1416,6 @@
       <c r="C11">
         <v>30</v>
       </c>
-      <c r="E11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11">
-        <v>20</v>
-      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1450,12 +1427,6 @@
       <c r="C12">
         <v>60</v>
       </c>
-      <c r="E12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12">
-        <v>30</v>
-      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1467,12 +1438,6 @@
       <c r="C13">
         <v>45</v>
       </c>
-      <c r="E13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13">
-        <v>45</v>
-      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1484,12 +1449,6 @@
       <c r="C14">
         <v>45</v>
       </c>
-      <c r="E14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14">
-        <v>45</v>
-      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1499,12 +1458,6 @@
         <v>19</v>
       </c>
       <c r="C15">
-        <v>120</v>
-      </c>
-      <c r="E15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15">
         <v>120</v>
       </c>
     </row>

</xml_diff>